<commit_message>
UPDATED FROM OFFICE 07072018
</commit_message>
<xml_diff>
--- a/Task_List.xlsx
+++ b/Task_List.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DGMU_DEBIT_TICKETING\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DGMU_System_Collection\AGC_DebitMemo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="46">
   <si>
     <t>PROGRESS</t>
   </si>
@@ -121,6 +121,48 @@
   </si>
   <si>
     <t>repDebitMemoTotalSummary_List_Supervisor</t>
+  </si>
+  <si>
+    <t>Create Personnel Maintenance</t>
+  </si>
+  <si>
+    <t>Create Dispatch Module</t>
+  </si>
+  <si>
+    <t>Dispatch Form</t>
+  </si>
+  <si>
+    <t>Hardware Requirement</t>
+  </si>
+  <si>
+    <t>Configure and setup server</t>
+  </si>
+  <si>
+    <t>This will server temporary server / specs is Workstation CPU</t>
+  </si>
+  <si>
+    <t>Deployment and Implementation of Debit Memo</t>
+  </si>
+  <si>
+    <t>Setup</t>
+  </si>
+  <si>
+    <t>Start of Debit Memo System</t>
+  </si>
+  <si>
+    <t>Need to start to be able to identify any concern and bugs.</t>
+  </si>
+  <si>
+    <t>Additional Voucher Module for Ma'am Anna</t>
+  </si>
+  <si>
+    <t>Voucher</t>
+  </si>
+  <si>
+    <t>Ms. Anna need to encode details for payment, requirement selection of Supplier to be paid.</t>
+  </si>
+  <si>
+    <t>It would be possible to have Supplier Maintenance</t>
   </si>
 </sst>
 </file>
@@ -607,8 +649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,7 +662,7 @@
     <col min="5" max="5" width="19.5703125" style="5" customWidth="1"/>
     <col min="6" max="6" width="15.5703125" style="5" customWidth="1"/>
     <col min="7" max="7" width="23.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24" style="19" customWidth="1"/>
+    <col min="8" max="8" width="23.85546875" style="19" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="39.5703125" customWidth="1"/>
     <col min="15" max="15" width="22.28515625" customWidth="1"/>
   </cols>
@@ -733,15 +775,17 @@
         <v>20</v>
       </c>
       <c r="D5" s="16">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F5" s="14">
         <v>43262</v>
       </c>
-      <c r="G5" s="12"/>
+      <c r="G5" s="20">
+        <v>43264</v>
+      </c>
       <c r="H5" s="18"/>
       <c r="I5" s="8"/>
     </row>
@@ -749,12 +793,24 @@
       <c r="A6" s="12">
         <v>5</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="12"/>
+      <c r="B6" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="16">
+        <v>1</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="14">
+        <v>43264</v>
+      </c>
+      <c r="G6" s="20">
+        <v>43265</v>
+      </c>
       <c r="H6" s="18"/>
       <c r="I6" s="8"/>
     </row>
@@ -762,59 +818,115 @@
       <c r="A7" s="12">
         <v>6</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="12"/>
+      <c r="B7" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="16">
+        <v>1</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="14">
+        <v>43269</v>
+      </c>
+      <c r="G7" s="20">
+        <v>43269</v>
+      </c>
       <c r="H7" s="18"/>
       <c r="I7" s="8"/>
     </row>
-    <row r="8" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>7</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="12"/>
+      <c r="B8" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="16">
+        <v>1</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="14">
+        <v>43286</v>
+      </c>
+      <c r="G8" s="20">
+        <v>43286</v>
+      </c>
       <c r="H8" s="18"/>
-      <c r="I8" s="8"/>
+      <c r="I8" s="8" t="s">
+        <v>37</v>
+      </c>
       <c r="O8" s="9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>8</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="8"/>
+      <c r="B9" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="16">
+        <v>1</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="14">
+        <v>43287</v>
+      </c>
+      <c r="G9" s="20">
+        <v>43287</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="I9" s="18" t="s">
+        <v>40</v>
+      </c>
       <c r="O9" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>9</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="14"/>
+      <c r="B10" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="14">
+        <v>43287</v>
+      </c>
       <c r="G10" s="12"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="8"/>
+      <c r="H10" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>45</v>
+      </c>
       <c r="O10" s="7" t="s">
         <v>11</v>
       </c>
@@ -1116,8 +1228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>